<commit_message>
Documents about DDS jitters added
</commit_message>
<xml_diff>
--- a/documents/波形相移现象记录.xlsx
+++ b/documents/波形相移现象记录.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programs\Verilog\FPGA_Group\test_br0101\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="11595"/>
   </bookViews>
@@ -101,19 +106,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -133,12 +138,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -147,11 +167,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -160,11 +183,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -206,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,9 +269,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,6 +321,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,14 +514,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
@@ -779,34 +846,34 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -817,12 +884,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -830,12 +897,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>